<commit_message>
added plotting for contact pressure metric.
</commit_message>
<xml_diff>
--- a/datalogs/Data Analysis/SummarySuccess.xlsx
+++ b/datalogs/Data Analysis/SummarySuccess.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravesh\Desktop\Research\FRR\FRR Software Interface\FRR-Software-Interface\datalogs\Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0BCDB5A3-D0C1-4FAF-8EA2-E1D302B15F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98DFDEE-2028-4802-AB23-BCC48CEE2655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,11 +21,24 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SummarySuccess!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId5"/>
-    <pivotCache cacheId="14" r:id="rId6"/>
+    <pivotCache cacheId="15" r:id="rId5"/>
+    <pivotCache cacheId="16" r:id="rId6"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -104,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -693,7 +706,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -702,18 +715,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -722,6 +731,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -995,6 +1007,118 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -1799,6 +1923,62 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -3482,7 +3662,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ravesh" refreshedDate="45159.682673958334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ravesh" refreshedDate="45159.682673958334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E24" sheet="SummarySuccess"/>
   </cacheSource>
@@ -3522,7 +3702,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ravesh" refreshedDate="45159.696267824074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ravesh" refreshedDate="45159.696267824074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF0E000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G24" sheet="SummarySuccess"/>
   </cacheSource>
@@ -3834,7 +4014,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:H7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -3977,7 +4157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -4120,7 +4300,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:H7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -4558,7 +4738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4623,25 +4803,25 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>8</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>13</v>
       </c>
     </row>
@@ -4649,17 +4829,13 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>2</v>
       </c>
     </row>
@@ -4667,25 +4843,25 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>11</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>21</v>
       </c>
     </row>
@@ -4693,25 +4869,25 @@
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>15</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>12</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>9</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>21</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>36</v>
       </c>
     </row>
@@ -4722,7 +4898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4769,14 +4945,13 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>21</v>
       </c>
     </row>
@@ -4784,14 +4959,13 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>12</v>
       </c>
     </row>
@@ -4799,14 +4973,13 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>6</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>9</v>
       </c>
     </row>
@@ -4814,16 +4987,16 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>12</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>26</v>
       </c>
     </row>
@@ -4831,16 +5004,16 @@
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>15</v>
       </c>
     </row>
@@ -4848,14 +5021,13 @@
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>11</v>
       </c>
     </row>
@@ -4863,16 +5035,16 @@
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>20</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>24</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>47</v>
       </c>
     </row>
@@ -4883,7 +5055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4902,45 +5074,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -4950,45 +5122,45 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -4998,22 +5170,22 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>2</f>
         <v>2</v>
       </c>
@@ -5023,45 +5195,45 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5071,22 +5243,22 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5096,22 +5268,22 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5121,22 +5293,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5146,22 +5318,22 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5171,45 +5343,45 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>0</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5219,22 +5391,22 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>3</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>2</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5244,45 +5416,45 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>0</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5292,22 +5464,22 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5317,68 +5489,68 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>3</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>0</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>3</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>0</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>4</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>1</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5388,22 +5560,22 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>3</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5413,45 +5585,45 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>4</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>0</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>2</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5461,22 +5633,22 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>4</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>3</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <f>3</f>
         <v>3</v>
       </c>
@@ -5486,30 +5658,30 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>4</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>0</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>0</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1">
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
       <sortCondition ref="C1"/>
     </sortState>
@@ -5519,11 +5691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5582,25 +5754,25 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>8</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>13</v>
       </c>
     </row>
@@ -5608,17 +5780,13 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>2</v>
       </c>
     </row>
@@ -5626,25 +5794,25 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>11</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>21</v>
       </c>
     </row>
@@ -5652,120 +5820,120 @@
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>15</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>12</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>9</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>21</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","SNS","Object Type","breakable")/5</f>
         <v>0.4</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="10">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","Manual","Object Type","breakable")/6</f>
         <v>0.5</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="13">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","SNS","Object Type","breakable")/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","Manual","Object Type","breakable")/6</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="16">
-        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","SNS","Object Type","fixed")/12</f>
+      <c r="B17" s="14">
+        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","SNS","Object Type","fixed")/6</f>
         <v>0</v>
       </c>
-      <c r="C17" s="13">
-        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","Manual","Object Type","fixed")/12</f>
+      <c r="C17" s="11">
+        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","Manual","Object Type","fixed")/6</f>
         <v>0</v>
       </c>
-      <c r="D17" s="16">
-        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","SNS","Object Type","fixed")/12</f>
+      <c r="D17" s="14">
+        <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","SNS","Object Type","fixed")/6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","Manual","Object Type","fixed")/6</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="15">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","SNS","Object Type","graspable")/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","Manual_first","Type of Control","Manual","Object Type","graspable")/6</f>
         <v>1</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="15">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","SNS","Object Type","graspable")/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <f>GETPIVOTDATA("Number of Successes",$A$1,"Group Type","SNS_first","Type of Control","Manual","Object Type","graspable")/6</f>
         <v>1</v>
       </c>

</xml_diff>